<commit_message>
Backup QR Scanner data - 2025-09-13T19:01:01.952Z - Cache Bust: 1757790061952
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_Dermatology_checklist1757789488840_backup@backdoor.com.xlsx
+++ b/log_history/Y4_B2526_Dermatology_checklist1757789488840_backup@backdoor.com.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Checklist" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -436,7 +436,7 @@
         <v>21:53:07</v>
       </c>
       <c r="E2" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F2" t="str">
         <v>backup@backdoor.com</v>
@@ -456,7 +456,7 @@
         <v>21:53:08</v>
       </c>
       <c r="E3" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F3" t="str">
         <v>backup@backdoor.com</v>
@@ -476,7 +476,7 @@
         <v>21:53:09</v>
       </c>
       <c r="E4" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F4" t="str">
         <v>backup@backdoor.com</v>
@@ -496,7 +496,7 @@
         <v>21:53:09</v>
       </c>
       <c r="E5" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F5" t="str">
         <v>backup@backdoor.com</v>
@@ -516,7 +516,7 @@
         <v>21:53:10</v>
       </c>
       <c r="E6" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F6" t="str">
         <v>backup@backdoor.com</v>

</xml_diff>

<commit_message>
Update edited session - 2025-09-13T19:02:11.696Z - Cache Bust ID: 1757790131696ocgupl9j8
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_Dermatology_checklist1757789488840_backup@backdoor.com.xlsx
+++ b/log_history/Y4_B2526_Dermatology_checklist1757789488840_backup@backdoor.com.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -502,29 +502,9 @@
         <v>backup@backdoor.com</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>220936</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C6" t="str">
-        <v>13/09/2025</v>
-      </c>
-      <c r="D6" t="str">
-        <v>21:53:10</v>
-      </c>
-      <c r="E6" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F6" t="str">
-        <v>backup@backdoor.com</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>